<commit_message>
custom subject add & add elective
</commit_message>
<xml_diff>
--- a/static/subjects.xlsx
+++ b/static/subjects.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\program\wed development\semeser\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A304E3-0B86-4B4A-B4EB-146028E83021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7FC10DC-4E38-4279-8B74-3971554FCF4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{82E6048D-3A5F-4860-856D-112B12198C03}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="8" xr2:uid="{82E6048D-3A5F-4860-856D-112B12198C03}"/>
   </bookViews>
   <sheets>
     <sheet name="semester1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,10 @@
     <sheet name="semester3" sheetId="3" r:id="rId3"/>
     <sheet name="semester4" sheetId="4" r:id="rId4"/>
     <sheet name="semester5" sheetId="5" r:id="rId5"/>
+    <sheet name="semester6" sheetId="7" r:id="rId6"/>
+    <sheet name="semester7" sheetId="8" r:id="rId7"/>
+    <sheet name="semester8" sheetId="9" r:id="rId8"/>
+    <sheet name="electives" sheetId="6" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="501">
   <si>
     <t>code</t>
   </si>
@@ -306,9 +310,6 @@
     <t>MX3084</t>
   </si>
   <si>
-    <t>DISASTER RISK REDUCTION AND MANAGEMENT</t>
-  </si>
-  <si>
     <t>SB8026</t>
   </si>
   <si>
@@ -316,6 +317,1236 @@
   </si>
   <si>
     <t>Web Technologies</t>
+  </si>
+  <si>
+    <t>CCS356</t>
+  </si>
+  <si>
+    <t>Object Oriented Software Engineering</t>
+  </si>
+  <si>
+    <t>CS3691</t>
+  </si>
+  <si>
+    <t>Embedded Systems and IoT</t>
+  </si>
+  <si>
+    <t>GE3791</t>
+  </si>
+  <si>
+    <t>Human Values and Ethics</t>
+  </si>
+  <si>
+    <t>CS3811</t>
+  </si>
+  <si>
+    <t>Project Work / Internship</t>
+  </si>
+  <si>
+    <t>GE3751</t>
+  </si>
+  <si>
+    <t>Principles of Management</t>
+  </si>
+  <si>
+    <t>GE3752</t>
+  </si>
+  <si>
+    <t>Total Quality Management</t>
+  </si>
+  <si>
+    <t>GE3753</t>
+  </si>
+  <si>
+    <t>Engineering Economics and Financial Accounting</t>
+  </si>
+  <si>
+    <t>GE3754</t>
+  </si>
+  <si>
+    <t>Human Resource Management</t>
+  </si>
+  <si>
+    <t>GE3755</t>
+  </si>
+  <si>
+    <t>Knowledge Management</t>
+  </si>
+  <si>
+    <t>GE3792</t>
+  </si>
+  <si>
+    <t>Industrial Management</t>
+  </si>
+  <si>
+    <t>MX3081</t>
+  </si>
+  <si>
+    <t>Introduction to Women and Gender Studies</t>
+  </si>
+  <si>
+    <t>MX3082</t>
+  </si>
+  <si>
+    <t>Elements of Literature</t>
+  </si>
+  <si>
+    <t>MX3083</t>
+  </si>
+  <si>
+    <t>Film Appreciation</t>
+  </si>
+  <si>
+    <t>Disaster Risk Reduction and Management</t>
+  </si>
+  <si>
+    <t>MX3085</t>
+  </si>
+  <si>
+    <t>Well Being with Traditional Practices – Yoga, Ayurveda and Siddha</t>
+  </si>
+  <si>
+    <t>MX3086</t>
+  </si>
+  <si>
+    <t>History of Science and Technology in India</t>
+  </si>
+  <si>
+    <t>MX3087</t>
+  </si>
+  <si>
+    <t>Political and Economic Thought for a Humane Society</t>
+  </si>
+  <si>
+    <t>MX3088</t>
+  </si>
+  <si>
+    <t>State, Nation Building and Politics in India</t>
+  </si>
+  <si>
+    <t>MX3089</t>
+  </si>
+  <si>
+    <t>Industrial Safety</t>
+  </si>
+  <si>
+    <t>CCS346</t>
+  </si>
+  <si>
+    <t>Exploratory Data Analysis</t>
+  </si>
+  <si>
+    <t>CCS360</t>
+  </si>
+  <si>
+    <t>Recommender Systems</t>
+  </si>
+  <si>
+    <t>CCS355</t>
+  </si>
+  <si>
+    <t>Neural Networks and Deep Learning</t>
+  </si>
+  <si>
+    <t>CCS369</t>
+  </si>
+  <si>
+    <t>Text and Speech Analysis</t>
+  </si>
+  <si>
+    <t>CCW331</t>
+  </si>
+  <si>
+    <t>Business Analytics</t>
+  </si>
+  <si>
+    <t>CCS349</t>
+  </si>
+  <si>
+    <t>Image and Video Analytics</t>
+  </si>
+  <si>
+    <t>CCS338</t>
+  </si>
+  <si>
+    <t>Computer Vision</t>
+  </si>
+  <si>
+    <t>CCS332</t>
+  </si>
+  <si>
+    <t>App Development</t>
+  </si>
+  <si>
+    <t>CCS336</t>
+  </si>
+  <si>
+    <t>Cloud Services Management</t>
+  </si>
+  <si>
+    <t>CCS370</t>
+  </si>
+  <si>
+    <t>UI and UX Design</t>
+  </si>
+  <si>
+    <t>CCS366</t>
+  </si>
+  <si>
+    <t>Software Testing and Automation</t>
+  </si>
+  <si>
+    <t>CCS374</t>
+  </si>
+  <si>
+    <t>Web Application Security</t>
+  </si>
+  <si>
+    <t>CCS342</t>
+  </si>
+  <si>
+    <t>DevOps</t>
+  </si>
+  <si>
+    <t>CCS358</t>
+  </si>
+  <si>
+    <t>Principles of Programming Languages</t>
+  </si>
+  <si>
+    <t>CCS335</t>
+  </si>
+  <si>
+    <t>Cloud Computing</t>
+  </si>
+  <si>
+    <t>CCS372</t>
+  </si>
+  <si>
+    <t>Virtualization</t>
+  </si>
+  <si>
+    <t>CCS341</t>
+  </si>
+  <si>
+    <t>Data Warehousing</t>
+  </si>
+  <si>
+    <t>CCS367</t>
+  </si>
+  <si>
+    <t>Storage Technologies</t>
+  </si>
+  <si>
+    <t>CCS365</t>
+  </si>
+  <si>
+    <t>Software Defined Networks</t>
+  </si>
+  <si>
+    <t>CCS368</t>
+  </si>
+  <si>
+    <t>Stream Processing</t>
+  </si>
+  <si>
+    <t>CCS362</t>
+  </si>
+  <si>
+    <t>Security and Privacy in Cloud</t>
+  </si>
+  <si>
+    <t>CCS344</t>
+  </si>
+  <si>
+    <t>Ethical Hacking</t>
+  </si>
+  <si>
+    <t>CCS343</t>
+  </si>
+  <si>
+    <t>Digital and Mobile Forensics</t>
+  </si>
+  <si>
+    <t>CCS363</t>
+  </si>
+  <si>
+    <t>Social Network Security</t>
+  </si>
+  <si>
+    <t>CCS351</t>
+  </si>
+  <si>
+    <t>Modern Cryptography</t>
+  </si>
+  <si>
+    <t>CB3591</t>
+  </si>
+  <si>
+    <t>Engineering Secure Software Systems</t>
+  </si>
+  <si>
+    <t>CCS339</t>
+  </si>
+  <si>
+    <t>Cryptocurrency and Blockchain Technologies</t>
+  </si>
+  <si>
+    <t>CCS354</t>
+  </si>
+  <si>
+    <t>Network Security</t>
+  </si>
+  <si>
+    <t>CCS333</t>
+  </si>
+  <si>
+    <t>Augmented Reality / Virtual Reality</t>
+  </si>
+  <si>
+    <t>CCS352</t>
+  </si>
+  <si>
+    <t>Multimedia and Animation</t>
+  </si>
+  <si>
+    <t>CCS371</t>
+  </si>
+  <si>
+    <t>Video Creation and Editing</t>
+  </si>
+  <si>
+    <t>CCW332</t>
+  </si>
+  <si>
+    <t>Digital Marketing</t>
+  </si>
+  <si>
+    <t>CCS373</t>
+  </si>
+  <si>
+    <t>Visual Effects</t>
+  </si>
+  <si>
+    <t>CCS347</t>
+  </si>
+  <si>
+    <t>Game Development</t>
+  </si>
+  <si>
+    <t>CCS353</t>
+  </si>
+  <si>
+    <t>Multimedia Data Compression and Storage</t>
+  </si>
+  <si>
+    <t>CCS361</t>
+  </si>
+  <si>
+    <t>Robotic Process Automation</t>
+  </si>
+  <si>
+    <t>CCS340</t>
+  </si>
+  <si>
+    <t>Cyber Security</t>
+  </si>
+  <si>
+    <t>CCS359</t>
+  </si>
+  <si>
+    <t>Quantum Computing</t>
+  </si>
+  <si>
+    <t>CCS331</t>
+  </si>
+  <si>
+    <t>3D Printing and Design</t>
+  </si>
+  <si>
+    <t>CCS350</t>
+  </si>
+  <si>
+    <t>Knowledge Engineering</t>
+  </si>
+  <si>
+    <t>CCS364</t>
+  </si>
+  <si>
+    <t>Soft Computing</t>
+  </si>
+  <si>
+    <t>CCS357</t>
+  </si>
+  <si>
+    <t>Optimization Techniques</t>
+  </si>
+  <si>
+    <t>CCS348</t>
+  </si>
+  <si>
+    <t>Game Theory</t>
+  </si>
+  <si>
+    <t>CCS337</t>
+  </si>
+  <si>
+    <t>Cognitive Science</t>
+  </si>
+  <si>
+    <t>CCS345</t>
+  </si>
+  <si>
+    <t>Ethics and AI</t>
+  </si>
+  <si>
+    <t>OAS351</t>
+  </si>
+  <si>
+    <t>Space Science</t>
+  </si>
+  <si>
+    <t>OIE351</t>
+  </si>
+  <si>
+    <t>Introduction to Industrial Engineering</t>
+  </si>
+  <si>
+    <t>OCE351</t>
+  </si>
+  <si>
+    <t>Environmental and Social Impact Assessment</t>
+  </si>
+  <si>
+    <t>OEE351</t>
+  </si>
+  <si>
+    <t>Renewable Energy System</t>
+  </si>
+  <si>
+    <t>OMA351</t>
+  </si>
+  <si>
+    <t>Graph Theory</t>
+  </si>
+  <si>
+    <t>OMG351</t>
+  </si>
+  <si>
+    <t>Fintech Regulation</t>
+  </si>
+  <si>
+    <t>OEI353</t>
+  </si>
+  <si>
+    <t>Introduction to PLC Programming</t>
+  </si>
+  <si>
+    <t>OCH351</t>
+  </si>
+  <si>
+    <t>Nano Technology</t>
+  </si>
+  <si>
+    <t>OPR351</t>
+  </si>
+  <si>
+    <t>Sustainable Manufacturing</t>
+  </si>
+  <si>
+    <t>OBT351</t>
+  </si>
+  <si>
+    <t>Food, Nutrition and Health</t>
+  </si>
+  <si>
+    <t>OEI351</t>
+  </si>
+  <si>
+    <t>Introduction to Industrial Instrumentation and Control</t>
+  </si>
+  <si>
+    <t>OIE352</t>
+  </si>
+  <si>
+    <t>Resource Management Techniques</t>
+  </si>
+  <si>
+    <t>OFD351</t>
+  </si>
+  <si>
+    <t>Holistic Nutrition</t>
+  </si>
+  <si>
+    <t>AI3021</t>
+  </si>
+  <si>
+    <t>IT in Agricultural System</t>
+  </si>
+  <si>
+    <t>OEI352</t>
+  </si>
+  <si>
+    <t>Introduction to Control Engineering</t>
+  </si>
+  <si>
+    <t>OPY351</t>
+  </si>
+  <si>
+    <t>Pharmaceutical Nanotechnology</t>
+  </si>
+  <si>
+    <t>OAE351</t>
+  </si>
+  <si>
+    <t>Aviation Management</t>
+  </si>
+  <si>
+    <t>OHS351</t>
+  </si>
+  <si>
+    <t>English for Competitive Examinations</t>
+  </si>
+  <si>
+    <t>OMG352</t>
+  </si>
+  <si>
+    <t>NGOs and Sustainable Development</t>
+  </si>
+  <si>
+    <t>OMG353</t>
+  </si>
+  <si>
+    <t>Democracy and Good Governance</t>
+  </si>
+  <si>
+    <t>CME365</t>
+  </si>
+  <si>
+    <t>Renewable Energy Technologies</t>
+  </si>
+  <si>
+    <t>OME354</t>
+  </si>
+  <si>
+    <t>Applied Design Thinking</t>
+  </si>
+  <si>
+    <t>MF3003</t>
+  </si>
+  <si>
+    <t>Reverse Engineering</t>
+  </si>
+  <si>
+    <t>AU3791</t>
+  </si>
+  <si>
+    <t>Electric and Hybrid Vehicles</t>
+  </si>
+  <si>
+    <t>OAS352</t>
+  </si>
+  <si>
+    <t>Space Engineering</t>
+  </si>
+  <si>
+    <t>OIM351</t>
+  </si>
+  <si>
+    <t>OIE354</t>
+  </si>
+  <si>
+    <t>Quality Engineering</t>
+  </si>
+  <si>
+    <t>OSF351</t>
+  </si>
+  <si>
+    <t>Fire Safety Engineering</t>
+  </si>
+  <si>
+    <t>OML351</t>
+  </si>
+  <si>
+    <t>Introduction to Non-destructive Testing</t>
+  </si>
+  <si>
+    <t>OMR351</t>
+  </si>
+  <si>
+    <t>Mechatronics</t>
+  </si>
+  <si>
+    <t>ORA351</t>
+  </si>
+  <si>
+    <t>Foundation of Robotics</t>
+  </si>
+  <si>
+    <t>OAE352</t>
+  </si>
+  <si>
+    <t>Fundamentals of Aeronautical Engineering</t>
+  </si>
+  <si>
+    <t>OGI351</t>
+  </si>
+  <si>
+    <t>Remote Sensing Concepts</t>
+  </si>
+  <si>
+    <t>OAI351</t>
+  </si>
+  <si>
+    <t>Urban Agriculture</t>
+  </si>
+  <si>
+    <t>OEN351</t>
+  </si>
+  <si>
+    <t>Drinking Water Supply and Treatment</t>
+  </si>
+  <si>
+    <t>OEE352</t>
+  </si>
+  <si>
+    <t>Electric Vehicle Technology</t>
+  </si>
+  <si>
+    <t>OCH352</t>
+  </si>
+  <si>
+    <t>Functional Materials</t>
+  </si>
+  <si>
+    <t>OFD352</t>
+  </si>
+  <si>
+    <t>Traditional Indian Foods</t>
+  </si>
+  <si>
+    <t>OFD353</t>
+  </si>
+  <si>
+    <t>Introduction to Food Processing</t>
+  </si>
+  <si>
+    <t>OPY352</t>
+  </si>
+  <si>
+    <t>IPR for Pharma Industry</t>
+  </si>
+  <si>
+    <t>OTT351</t>
+  </si>
+  <si>
+    <t>Basics of Textile Finishing</t>
+  </si>
+  <si>
+    <t>OTT352</t>
+  </si>
+  <si>
+    <t>Industrial Engineering for Garment Industry</t>
+  </si>
+  <si>
+    <t>OTT353</t>
+  </si>
+  <si>
+    <t>Basics of Textile Manufacture</t>
+  </si>
+  <si>
+    <t>OPE351</t>
+  </si>
+  <si>
+    <t>Introduction to Petroleum Refining and Petrochemicals</t>
+  </si>
+  <si>
+    <t>CPE334</t>
+  </si>
+  <si>
+    <t>Energy Conservation and Management</t>
+  </si>
+  <si>
+    <t>OPT351</t>
+  </si>
+  <si>
+    <t>Basics of Plastics Processing</t>
+  </si>
+  <si>
+    <t>OEC351</t>
+  </si>
+  <si>
+    <t>Signals and Systems</t>
+  </si>
+  <si>
+    <t>OEC352</t>
+  </si>
+  <si>
+    <t>Fundamentals of Electronic Devices and Circuits</t>
+  </si>
+  <si>
+    <t>CBM348</t>
+  </si>
+  <si>
+    <t>Foundation Skills in Integrated Product Development</t>
+  </si>
+  <si>
+    <t>CBM333</t>
+  </si>
+  <si>
+    <t>Assistive Technology</t>
+  </si>
+  <si>
+    <t>OMA352</t>
+  </si>
+  <si>
+    <t>Operations Research</t>
+  </si>
+  <si>
+    <t>OMA353</t>
+  </si>
+  <si>
+    <t>Algebra and Number Theory</t>
+  </si>
+  <si>
+    <t>OMA354</t>
+  </si>
+  <si>
+    <t>Linear Algebra</t>
+  </si>
+  <si>
+    <t>OCE353</t>
+  </si>
+  <si>
+    <t>Lean Concepts, Tools and Practices</t>
+  </si>
+  <si>
+    <t>OBT352</t>
+  </si>
+  <si>
+    <t>Basics of Microbial Technology</t>
+  </si>
+  <si>
+    <t>OBT353</t>
+  </si>
+  <si>
+    <t>Basics of Biomolecules</t>
+  </si>
+  <si>
+    <t>OBT354</t>
+  </si>
+  <si>
+    <t>Fundamentals of Cell and Molecular Biology</t>
+  </si>
+  <si>
+    <t>OHS352</t>
+  </si>
+  <si>
+    <t>Project Report Writing</t>
+  </si>
+  <si>
+    <t>OMA355</t>
+  </si>
+  <si>
+    <t>Advanced Numerical Methods</t>
+  </si>
+  <si>
+    <t>OMA356</t>
+  </si>
+  <si>
+    <t>Random Processes</t>
+  </si>
+  <si>
+    <t>OMA357</t>
+  </si>
+  <si>
+    <t>Queuing and Reliability Modelling</t>
+  </si>
+  <si>
+    <t>OMG354</t>
+  </si>
+  <si>
+    <t>Production and Operations Management for Entrepreneurs</t>
+  </si>
+  <si>
+    <t>OMG355</t>
+  </si>
+  <si>
+    <t>Multivariate Data Analysis</t>
+  </si>
+  <si>
+    <t>OME352</t>
+  </si>
+  <si>
+    <t>Additive Manufacturing</t>
+  </si>
+  <si>
+    <t>CME343</t>
+  </si>
+  <si>
+    <t>New Product Development</t>
+  </si>
+  <si>
+    <t>OME355</t>
+  </si>
+  <si>
+    <t>Industrial Design &amp; Rapid Prototyping Techniques</t>
+  </si>
+  <si>
+    <t>MF3010</t>
+  </si>
+  <si>
+    <t>Micro and Precision Engineering</t>
+  </si>
+  <si>
+    <t>OMF354</t>
+  </si>
+  <si>
+    <t>Cost Management of Engineering Projects</t>
+  </si>
+  <si>
+    <t>AU3002</t>
+  </si>
+  <si>
+    <t>Batteries and Management System</t>
+  </si>
+  <si>
+    <t>AU3008</t>
+  </si>
+  <si>
+    <t>Sensors and Actuators</t>
+  </si>
+  <si>
+    <t>OAS353</t>
+  </si>
+  <si>
+    <t>Space Vehicles</t>
+  </si>
+  <si>
+    <t>OIM352</t>
+  </si>
+  <si>
+    <t>Management Science</t>
+  </si>
+  <si>
+    <t>OIM353</t>
+  </si>
+  <si>
+    <t>Production Planning and Control</t>
+  </si>
+  <si>
+    <t>OIE353</t>
+  </si>
+  <si>
+    <t>Operations Management</t>
+  </si>
+  <si>
+    <t>OSF352</t>
+  </si>
+  <si>
+    <t>Industrial Hygiene</t>
+  </si>
+  <si>
+    <t>OSF353</t>
+  </si>
+  <si>
+    <t>Chemical Process Safety</t>
+  </si>
+  <si>
+    <t>OML352</t>
+  </si>
+  <si>
+    <t>Electrical, Electronic and Magnetic Materials</t>
+  </si>
+  <si>
+    <t>OML353</t>
+  </si>
+  <si>
+    <t>Nanomaterials and Applications</t>
+  </si>
+  <si>
+    <t>OMR352</t>
+  </si>
+  <si>
+    <t>Hydraulics and Pneumatics</t>
+  </si>
+  <si>
+    <t>OMR353</t>
+  </si>
+  <si>
+    <t>Sensors</t>
+  </si>
+  <si>
+    <t>ORA352</t>
+  </si>
+  <si>
+    <t>Concepts in Mobile Robots</t>
+  </si>
+  <si>
+    <t>MV3501</t>
+  </si>
+  <si>
+    <t>Marine Propulsion</t>
+  </si>
+  <si>
+    <t>OMV351</t>
+  </si>
+  <si>
+    <t>Marine Merchant Vessels</t>
+  </si>
+  <si>
+    <t>OMV352</t>
+  </si>
+  <si>
+    <t>Elements of Marine Engineering</t>
+  </si>
+  <si>
+    <t>CRA332</t>
+  </si>
+  <si>
+    <t>Drone Technologies</t>
+  </si>
+  <si>
+    <t>OGI352</t>
+  </si>
+  <si>
+    <t>Geographical Information System</t>
+  </si>
+  <si>
+    <t>OAI352</t>
+  </si>
+  <si>
+    <t>Agriculture Entrepreneurship Development</t>
+  </si>
+  <si>
+    <t>OEN352</t>
+  </si>
+  <si>
+    <t>Biodiversity Conservation</t>
+  </si>
+  <si>
+    <t>OEE353</t>
+  </si>
+  <si>
+    <t>Introduction to Control Systems</t>
+  </si>
+  <si>
+    <t>OEI354</t>
+  </si>
+  <si>
+    <t>Introduction to Industrial Automation Systems</t>
+  </si>
+  <si>
+    <t>OCH353</t>
+  </si>
+  <si>
+    <t>Energy Technology</t>
+  </si>
+  <si>
+    <t>OCH354</t>
+  </si>
+  <si>
+    <t>Surface Science</t>
+  </si>
+  <si>
+    <t>OFD354</t>
+  </si>
+  <si>
+    <t>Fundamentals of Food Engineering</t>
+  </si>
+  <si>
+    <t>OFD355</t>
+  </si>
+  <si>
+    <t>Food Safety and Quality Regulations</t>
+  </si>
+  <si>
+    <t>OPY353</t>
+  </si>
+  <si>
+    <t>Nutraceuticals</t>
+  </si>
+  <si>
+    <t>OTT354</t>
+  </si>
+  <si>
+    <t>Basics of Dyeing and Printing</t>
+  </si>
+  <si>
+    <t>FT3201</t>
+  </si>
+  <si>
+    <t>Fibre Science</t>
+  </si>
+  <si>
+    <t>OTT355</t>
+  </si>
+  <si>
+    <t>Garment Manufacturing Technology</t>
+  </si>
+  <si>
+    <t>OPE353</t>
+  </si>
+  <si>
+    <t>OPE354</t>
+  </si>
+  <si>
+    <t>Unit Operations in Petro Chemical Industries</t>
+  </si>
+  <si>
+    <t>OPT352</t>
+  </si>
+  <si>
+    <t>Plastic Materials for Engineers</t>
+  </si>
+  <si>
+    <t>OPT353</t>
+  </si>
+  <si>
+    <t>Properties and Testing of Plastics</t>
+  </si>
+  <si>
+    <t>OEC353</t>
+  </si>
+  <si>
+    <t>VLSI Design</t>
+  </si>
+  <si>
+    <t>CBM370</t>
+  </si>
+  <si>
+    <t>Wearable Devices</t>
+  </si>
+  <si>
+    <t>CBM356</t>
+  </si>
+  <si>
+    <t>Medical Informatics</t>
+  </si>
+  <si>
+    <t>OCE354</t>
+  </si>
+  <si>
+    <t>Basics of Integrated Water Resources Management</t>
+  </si>
+  <si>
+    <t>OBT355</t>
+  </si>
+  <si>
+    <t>Biotechnology for Waste Management</t>
+  </si>
+  <si>
+    <t>OBT356</t>
+  </si>
+  <si>
+    <t>Lifestyle Diseases</t>
+  </si>
+  <si>
+    <t>OBT357</t>
+  </si>
+  <si>
+    <t>Biotechnology in Health Care</t>
+  </si>
+  <si>
+    <t>CMG331</t>
+  </si>
+  <si>
+    <t>Financial Management</t>
+  </si>
+  <si>
+    <t>CMG332</t>
+  </si>
+  <si>
+    <t>Fundamentals of Investment</t>
+  </si>
+  <si>
+    <t>CMG333</t>
+  </si>
+  <si>
+    <t>Banking, Financial Services and Insurance</t>
+  </si>
+  <si>
+    <t>CMG334</t>
+  </si>
+  <si>
+    <t>Introduction to Blockchain and its Applications</t>
+  </si>
+  <si>
+    <t>CMG335</t>
+  </si>
+  <si>
+    <t>Fintech Personal Finance and Payments</t>
+  </si>
+  <si>
+    <t>CMG336</t>
+  </si>
+  <si>
+    <t>Introduction to Fintech</t>
+  </si>
+  <si>
+    <t>CMG337</t>
+  </si>
+  <si>
+    <t>Foundations of Entrepreneurship</t>
+  </si>
+  <si>
+    <t>CMG338</t>
+  </si>
+  <si>
+    <t>Team Building &amp; Leadership Management for Business</t>
+  </si>
+  <si>
+    <t>CMG339</t>
+  </si>
+  <si>
+    <t>Creativity &amp; Innovation in Entrepreneurship</t>
+  </si>
+  <si>
+    <t>CMG340</t>
+  </si>
+  <si>
+    <t>Principles of Marketing Management For Business</t>
+  </si>
+  <si>
+    <t>CMG341</t>
+  </si>
+  <si>
+    <t>Human Resource Management for Entrepreneurs</t>
+  </si>
+  <si>
+    <t>CMG342</t>
+  </si>
+  <si>
+    <t>Financing New Business Ventures</t>
+  </si>
+  <si>
+    <t>CMG343</t>
+  </si>
+  <si>
+    <t>Principles of Public Administration</t>
+  </si>
+  <si>
+    <t>CMG344</t>
+  </si>
+  <si>
+    <t>Constitution of India</t>
+  </si>
+  <si>
+    <t>CMG345</t>
+  </si>
+  <si>
+    <t>Public Personnel Administration</t>
+  </si>
+  <si>
+    <t>CMG346</t>
+  </si>
+  <si>
+    <t>Administrative Theories</t>
+  </si>
+  <si>
+    <t>CMG347</t>
+  </si>
+  <si>
+    <t>Indian Administrative System</t>
+  </si>
+  <si>
+    <t>CMG348</t>
+  </si>
+  <si>
+    <t>Public Policy Administration</t>
+  </si>
+  <si>
+    <t>CMG349</t>
+  </si>
+  <si>
+    <t>Statistics for Management</t>
+  </si>
+  <si>
+    <t>CMG350</t>
+  </si>
+  <si>
+    <t>Datamining For Business Intelligence</t>
+  </si>
+  <si>
+    <t>CMG351</t>
+  </si>
+  <si>
+    <t>Human Resource Analytics</t>
+  </si>
+  <si>
+    <t>CMG352</t>
+  </si>
+  <si>
+    <t>Marketing and Social Media Web Analytics</t>
+  </si>
+  <si>
+    <t>CMG353</t>
+  </si>
+  <si>
+    <t>Operation and Supply Chain Analytics</t>
+  </si>
+  <si>
+    <t>CMG354</t>
+  </si>
+  <si>
+    <t>Financial Analytics</t>
+  </si>
+  <si>
+    <t>CES331</t>
+  </si>
+  <si>
+    <t>Sustainable Infrastructure Development</t>
+  </si>
+  <si>
+    <t>CES332</t>
+  </si>
+  <si>
+    <t>Sustainable Agriculture and Environmental Management</t>
+  </si>
+  <si>
+    <t>CES333</t>
+  </si>
+  <si>
+    <t>Sustainable Bio Materials</t>
+  </si>
+  <si>
+    <t>CES334</t>
+  </si>
+  <si>
+    <t>Materials for Energy Sustainability</t>
+  </si>
+  <si>
+    <t>CES335</t>
+  </si>
+  <si>
+    <t>Green Technology</t>
+  </si>
+  <si>
+    <t>CES336</t>
+  </si>
+  <si>
+    <t>Environmental Quality Monitoring and Analysis</t>
+  </si>
+  <si>
+    <t>CES337</t>
+  </si>
+  <si>
+    <t>Integrated Energy Planning for Sustainable Development</t>
+  </si>
+  <si>
+    <t>CES338</t>
+  </si>
+  <si>
+    <t>Energy Efficiency for Sustainable Development</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CS3711 </t>
+  </si>
+  <si>
+    <t>Summer internship</t>
+  </si>
+  <si>
+    <t>NM3000</t>
   </si>
 </sst>
 </file>
@@ -359,7 +1590,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -369,6 +1600,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1086,7 +2323,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1211,10 +2448,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3207A2B-C456-4C25-A2AA-16916F6DD8B7}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1281,49 +2518,2537 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B6" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="C6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>86</v>
-      </c>
-      <c r="B7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>87</v>
-      </c>
-      <c r="B8" t="s">
-        <v>88</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>89</v>
-      </c>
-      <c r="B9" t="s">
-        <v>76</v>
-      </c>
-      <c r="C9">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF255841-3112-4694-912C-A985050C35C8}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.88671875" customWidth="1"/>
+    <col min="2" max="2" width="33.21875" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FB14740-2706-422C-9FE6-817F03681B57}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="29.33203125" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>498</v>
+      </c>
+      <c r="B3" t="s">
+        <v>499</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6205CC0A-78C0-4052-BB3C-D90135036E83}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="32" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2A96EBE-7B3F-4BF2-9E1C-04C296420266}">
+  <dimension ref="A1:C214"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="33.6640625" customWidth="1"/>
+    <col min="2" max="2" width="42.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>500</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C8" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C18" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C19" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C20" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C21" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C22" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C23" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C24" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C26" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C27" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C28" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C29" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C30" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C31" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C32" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C33" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C34" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C35" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C36" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C37" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C38" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C39" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C40" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C41" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C42" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C43" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C44" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C45" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C46" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C47" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C48" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C49" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C50" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C51" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C52" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C53" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C54" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C55" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C56" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C57" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C58" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C59" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C60" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C61" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C62" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C63" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C64" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C65" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C66" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C67" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C68" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C69" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C70" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C71" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C72" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C73" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>218</v>
+      </c>
+      <c r="B74" t="s">
+        <v>219</v>
+      </c>
+      <c r="C74">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>220</v>
+      </c>
+      <c r="B75" t="s">
+        <v>221</v>
+      </c>
+      <c r="C75">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>236</v>
+      </c>
+      <c r="B76" t="s">
+        <v>237</v>
+      </c>
+      <c r="C76">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>222</v>
+      </c>
+      <c r="B77" t="s">
+        <v>223</v>
+      </c>
+      <c r="C77">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>224</v>
+      </c>
+      <c r="B78" t="s">
+        <v>225</v>
+      </c>
+      <c r="C78">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>238</v>
+      </c>
+      <c r="B79" t="s">
+        <v>239</v>
+      </c>
+      <c r="C79">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>226</v>
+      </c>
+      <c r="B80" t="s">
+        <v>227</v>
+      </c>
+      <c r="C80">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>240</v>
+      </c>
+      <c r="B81" t="s">
+        <v>241</v>
+      </c>
+      <c r="C81">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>228</v>
+      </c>
+      <c r="B82" t="s">
+        <v>229</v>
+      </c>
+      <c r="C82">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>242</v>
+      </c>
+      <c r="B83" t="s">
+        <v>243</v>
+      </c>
+      <c r="C83">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>244</v>
+      </c>
+      <c r="B84" t="s">
+        <v>245</v>
+      </c>
+      <c r="C84">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>246</v>
+      </c>
+      <c r="B85" t="s">
+        <v>247</v>
+      </c>
+      <c r="C85">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>248</v>
+      </c>
+      <c r="B86" t="s">
+        <v>249</v>
+      </c>
+      <c r="C86">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>250</v>
+      </c>
+      <c r="B87" t="s">
+        <v>251</v>
+      </c>
+      <c r="C87">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>252</v>
+      </c>
+      <c r="B88" t="s">
+        <v>253</v>
+      </c>
+      <c r="C88">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>254</v>
+      </c>
+      <c r="B89" t="s">
+        <v>255</v>
+      </c>
+      <c r="C89">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>256</v>
+      </c>
+      <c r="B90" t="s">
+        <v>257</v>
+      </c>
+      <c r="C90">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>258</v>
+      </c>
+      <c r="B91" t="s">
+        <v>259</v>
+      </c>
+      <c r="C91">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>260</v>
+      </c>
+      <c r="B92" t="s">
+        <v>261</v>
+      </c>
+      <c r="C92">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>262</v>
+      </c>
+      <c r="B93" t="s">
+        <v>263</v>
+      </c>
+      <c r="C93">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>234</v>
+      </c>
+      <c r="B94" t="s">
+        <v>235</v>
+      </c>
+      <c r="C94">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>264</v>
+      </c>
+      <c r="B95" t="s">
+        <v>265</v>
+      </c>
+      <c r="C95">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>266</v>
+      </c>
+      <c r="B96" t="s">
+        <v>267</v>
+      </c>
+      <c r="C96">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>268</v>
+      </c>
+      <c r="B97" t="s">
+        <v>110</v>
+      </c>
+      <c r="C97">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>269</v>
+      </c>
+      <c r="B98" t="s">
+        <v>270</v>
+      </c>
+      <c r="C98">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>271</v>
+      </c>
+      <c r="B99" t="s">
+        <v>272</v>
+      </c>
+      <c r="C99">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>273</v>
+      </c>
+      <c r="B100" t="s">
+        <v>274</v>
+      </c>
+      <c r="C100">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>275</v>
+      </c>
+      <c r="B101" t="s">
+        <v>276</v>
+      </c>
+      <c r="C101">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>277</v>
+      </c>
+      <c r="B102" t="s">
+        <v>278</v>
+      </c>
+      <c r="C102">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>279</v>
+      </c>
+      <c r="B103" t="s">
+        <v>280</v>
+      </c>
+      <c r="C103">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>281</v>
+      </c>
+      <c r="B104" t="s">
+        <v>282</v>
+      </c>
+      <c r="C104">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>283</v>
+      </c>
+      <c r="B105" t="s">
+        <v>284</v>
+      </c>
+      <c r="C105">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>285</v>
+      </c>
+      <c r="B106" t="s">
+        <v>286</v>
+      </c>
+      <c r="C106">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>287</v>
+      </c>
+      <c r="B107" t="s">
+        <v>288</v>
+      </c>
+      <c r="C107">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>230</v>
+      </c>
+      <c r="B108" t="s">
+        <v>231</v>
+      </c>
+      <c r="C108">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>232</v>
+      </c>
+      <c r="B109" t="s">
+        <v>233</v>
+      </c>
+      <c r="C109">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>289</v>
+      </c>
+      <c r="B110" t="s">
+        <v>290</v>
+      </c>
+      <c r="C110">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>291</v>
+      </c>
+      <c r="B111" t="s">
+        <v>292</v>
+      </c>
+      <c r="C111">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>293</v>
+      </c>
+      <c r="B112" t="s">
+        <v>294</v>
+      </c>
+      <c r="C112">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>295</v>
+      </c>
+      <c r="B113" t="s">
+        <v>296</v>
+      </c>
+      <c r="C113">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>297</v>
+      </c>
+      <c r="B114" t="s">
+        <v>298</v>
+      </c>
+      <c r="C114">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>299</v>
+      </c>
+      <c r="B115" t="s">
+        <v>300</v>
+      </c>
+      <c r="C115">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>301</v>
+      </c>
+      <c r="B116" t="s">
+        <v>302</v>
+      </c>
+      <c r="C116">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>303</v>
+      </c>
+      <c r="B117" t="s">
+        <v>304</v>
+      </c>
+      <c r="C117">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>305</v>
+      </c>
+      <c r="B118" t="s">
+        <v>306</v>
+      </c>
+      <c r="C118">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>307</v>
+      </c>
+      <c r="B119" t="s">
+        <v>308</v>
+      </c>
+      <c r="C119">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>309</v>
+      </c>
+      <c r="B120" t="s">
+        <v>310</v>
+      </c>
+      <c r="C120">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>311</v>
+      </c>
+      <c r="B121" t="s">
+        <v>312</v>
+      </c>
+      <c r="C121">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>313</v>
+      </c>
+      <c r="B122" t="s">
+        <v>314</v>
+      </c>
+      <c r="C122">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>315</v>
+      </c>
+      <c r="B123" t="s">
+        <v>316</v>
+      </c>
+      <c r="C123">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>317</v>
+      </c>
+      <c r="B124" t="s">
+        <v>318</v>
+      </c>
+      <c r="C124">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>319</v>
+      </c>
+      <c r="B125" t="s">
+        <v>320</v>
+      </c>
+      <c r="C125">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>321</v>
+      </c>
+      <c r="B126" t="s">
+        <v>322</v>
+      </c>
+      <c r="C126">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>323</v>
+      </c>
+      <c r="B127" t="s">
+        <v>324</v>
+      </c>
+      <c r="C127">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>325</v>
+      </c>
+      <c r="B128" t="s">
+        <v>326</v>
+      </c>
+      <c r="C128">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>327</v>
+      </c>
+      <c r="B129" t="s">
+        <v>328</v>
+      </c>
+      <c r="C129">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>329</v>
+      </c>
+      <c r="B130" t="s">
+        <v>330</v>
+      </c>
+      <c r="C130">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
+        <v>331</v>
+      </c>
+      <c r="B131" t="s">
+        <v>332</v>
+      </c>
+      <c r="C131">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>333</v>
+      </c>
+      <c r="B132" t="s">
+        <v>334</v>
+      </c>
+      <c r="C132">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>335</v>
+      </c>
+      <c r="B133" t="s">
+        <v>336</v>
+      </c>
+      <c r="C133">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>337</v>
+      </c>
+      <c r="B134" t="s">
+        <v>338</v>
+      </c>
+      <c r="C134">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>339</v>
+      </c>
+      <c r="B135" t="s">
+        <v>340</v>
+      </c>
+      <c r="C135">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>341</v>
+      </c>
+      <c r="B136" t="s">
+        <v>342</v>
+      </c>
+      <c r="C136">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>343</v>
+      </c>
+      <c r="B137" t="s">
+        <v>344</v>
+      </c>
+      <c r="C137">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>345</v>
+      </c>
+      <c r="B138" t="s">
+        <v>346</v>
+      </c>
+      <c r="C138">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
+        <v>347</v>
+      </c>
+      <c r="B139" t="s">
+        <v>348</v>
+      </c>
+      <c r="C139">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>349</v>
+      </c>
+      <c r="B140" t="s">
+        <v>350</v>
+      </c>
+      <c r="C140">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>351</v>
+      </c>
+      <c r="B141" t="s">
+        <v>352</v>
+      </c>
+      <c r="C141">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
+        <v>353</v>
+      </c>
+      <c r="B142" t="s">
+        <v>354</v>
+      </c>
+      <c r="C142">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
+        <v>355</v>
+      </c>
+      <c r="B143" t="s">
+        <v>356</v>
+      </c>
+      <c r="C143">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
+        <v>357</v>
+      </c>
+      <c r="B144" t="s">
+        <v>358</v>
+      </c>
+      <c r="C144">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>359</v>
+      </c>
+      <c r="B145" t="s">
+        <v>360</v>
+      </c>
+      <c r="C145">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
+        <v>361</v>
+      </c>
+      <c r="B146" t="s">
+        <v>362</v>
+      </c>
+      <c r="C146">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
+        <v>363</v>
+      </c>
+      <c r="B147" t="s">
+        <v>364</v>
+      </c>
+      <c r="C147">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
+        <v>365</v>
+      </c>
+      <c r="B148" t="s">
+        <v>366</v>
+      </c>
+      <c r="C148">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
+        <v>367</v>
+      </c>
+      <c r="B149" t="s">
+        <v>368</v>
+      </c>
+      <c r="C149">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
+        <v>369</v>
+      </c>
+      <c r="B150" t="s">
+        <v>370</v>
+      </c>
+      <c r="C150">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
+        <v>371</v>
+      </c>
+      <c r="B151" t="s">
+        <v>372</v>
+      </c>
+      <c r="C151">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
+        <v>373</v>
+      </c>
+      <c r="B152" t="s">
+        <v>374</v>
+      </c>
+      <c r="C152">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A153" t="s">
+        <v>375</v>
+      </c>
+      <c r="B153" t="s">
+        <v>376</v>
+      </c>
+      <c r="C153">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A154" t="s">
+        <v>377</v>
+      </c>
+      <c r="B154" t="s">
+        <v>378</v>
+      </c>
+      <c r="C154">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A155" t="s">
+        <v>379</v>
+      </c>
+      <c r="B155" t="s">
+        <v>380</v>
+      </c>
+      <c r="C155">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A156" t="s">
+        <v>381</v>
+      </c>
+      <c r="B156" t="s">
+        <v>382</v>
+      </c>
+      <c r="C156">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A157" t="s">
+        <v>383</v>
+      </c>
+      <c r="B157" t="s">
+        <v>384</v>
+      </c>
+      <c r="C157">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A158" t="s">
+        <v>385</v>
+      </c>
+      <c r="B158" t="s">
+        <v>386</v>
+      </c>
+      <c r="C158">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A159" t="s">
+        <v>387</v>
+      </c>
+      <c r="B159" t="s">
+        <v>388</v>
+      </c>
+      <c r="C159">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A160" t="s">
+        <v>389</v>
+      </c>
+      <c r="B160" t="s">
+        <v>390</v>
+      </c>
+      <c r="C160">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A161" t="s">
+        <v>391</v>
+      </c>
+      <c r="B161" t="s">
+        <v>392</v>
+      </c>
+      <c r="C161">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A162" t="s">
+        <v>393</v>
+      </c>
+      <c r="B162" t="s">
+        <v>394</v>
+      </c>
+      <c r="C162">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A163" t="s">
+        <v>395</v>
+      </c>
+      <c r="B163" t="s">
+        <v>396</v>
+      </c>
+      <c r="C163">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A164" t="s">
+        <v>397</v>
+      </c>
+      <c r="B164" t="s">
+        <v>398</v>
+      </c>
+      <c r="C164">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A165" t="s">
+        <v>399</v>
+      </c>
+      <c r="B165" t="s">
+        <v>400</v>
+      </c>
+      <c r="C165">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A166" t="s">
+        <v>401</v>
+      </c>
+      <c r="B166" t="s">
+        <v>402</v>
+      </c>
+      <c r="C166">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A167" t="s">
+        <v>403</v>
+      </c>
+      <c r="B167" t="s">
+        <v>404</v>
+      </c>
+      <c r="C167">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A168" t="s">
+        <v>405</v>
+      </c>
+      <c r="B168" t="s">
+        <v>406</v>
+      </c>
+      <c r="C168">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A169" t="s">
+        <v>407</v>
+      </c>
+      <c r="B169" t="s">
+        <v>408</v>
+      </c>
+      <c r="C169">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A170" t="s">
+        <v>409</v>
+      </c>
+      <c r="B170" t="s">
+        <v>410</v>
+      </c>
+      <c r="C170">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A171" t="s">
+        <v>411</v>
+      </c>
+      <c r="B171" t="s">
+        <v>412</v>
+      </c>
+      <c r="C171">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A172" t="s">
+        <v>413</v>
+      </c>
+      <c r="B172" t="s">
+        <v>127</v>
+      </c>
+      <c r="C172">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A173" t="s">
+        <v>414</v>
+      </c>
+      <c r="B173" t="s">
+        <v>415</v>
+      </c>
+      <c r="C173">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A174" t="s">
+        <v>416</v>
+      </c>
+      <c r="B174" t="s">
+        <v>417</v>
+      </c>
+      <c r="C174">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A175" t="s">
+        <v>418</v>
+      </c>
+      <c r="B175" t="s">
+        <v>419</v>
+      </c>
+      <c r="C175">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A176" t="s">
+        <v>420</v>
+      </c>
+      <c r="B176" t="s">
+        <v>421</v>
+      </c>
+      <c r="C176">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A177" t="s">
+        <v>422</v>
+      </c>
+      <c r="B177" t="s">
+        <v>423</v>
+      </c>
+      <c r="C177">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A178" t="s">
+        <v>424</v>
+      </c>
+      <c r="B178" t="s">
+        <v>425</v>
+      </c>
+      <c r="C178">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A179" t="s">
+        <v>426</v>
+      </c>
+      <c r="B179" t="s">
+        <v>427</v>
+      </c>
+      <c r="C179">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A180" t="s">
+        <v>428</v>
+      </c>
+      <c r="B180" t="s">
+        <v>429</v>
+      </c>
+      <c r="C180">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A181" t="s">
+        <v>430</v>
+      </c>
+      <c r="B181" t="s">
+        <v>431</v>
+      </c>
+      <c r="C181">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A182" t="s">
+        <v>432</v>
+      </c>
+      <c r="B182" t="s">
+        <v>433</v>
+      </c>
+      <c r="C182">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A183" t="s">
+        <v>434</v>
+      </c>
+      <c r="B183" t="s">
+        <v>435</v>
+      </c>
+      <c r="C183">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A184" t="s">
+        <v>436</v>
+      </c>
+      <c r="B184" t="s">
+        <v>437</v>
+      </c>
+      <c r="C184">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A185" t="s">
+        <v>438</v>
+      </c>
+      <c r="B185" t="s">
+        <v>439</v>
+      </c>
+      <c r="C185">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A186" t="s">
+        <v>440</v>
+      </c>
+      <c r="B186" t="s">
+        <v>441</v>
+      </c>
+      <c r="C186">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A187" t="s">
+        <v>442</v>
+      </c>
+      <c r="B187" t="s">
+        <v>443</v>
+      </c>
+      <c r="C187">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A188" t="s">
+        <v>444</v>
+      </c>
+      <c r="B188" t="s">
+        <v>445</v>
+      </c>
+      <c r="C188">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A189" t="s">
+        <v>446</v>
+      </c>
+      <c r="B189" t="s">
+        <v>447</v>
+      </c>
+      <c r="C189">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A190" t="s">
+        <v>448</v>
+      </c>
+      <c r="B190" t="s">
+        <v>449</v>
+      </c>
+      <c r="C190">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A191" t="s">
+        <v>450</v>
+      </c>
+      <c r="B191" t="s">
+        <v>451</v>
+      </c>
+      <c r="C191">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A192" t="s">
+        <v>452</v>
+      </c>
+      <c r="B192" t="s">
+        <v>453</v>
+      </c>
+      <c r="C192">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A193" t="s">
+        <v>454</v>
+      </c>
+      <c r="B193" t="s">
+        <v>455</v>
+      </c>
+      <c r="C193">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A194" t="s">
+        <v>456</v>
+      </c>
+      <c r="B194" t="s">
+        <v>457</v>
+      </c>
+      <c r="C194">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A195" t="s">
+        <v>458</v>
+      </c>
+      <c r="B195" t="s">
+        <v>459</v>
+      </c>
+      <c r="C195">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A196" t="s">
+        <v>460</v>
+      </c>
+      <c r="B196" t="s">
+        <v>461</v>
+      </c>
+      <c r="C196">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A197" t="s">
+        <v>462</v>
+      </c>
+      <c r="B197" t="s">
+        <v>463</v>
+      </c>
+      <c r="C197">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A198" t="s">
+        <v>464</v>
+      </c>
+      <c r="B198" t="s">
+        <v>465</v>
+      </c>
+      <c r="C198">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A199" t="s">
+        <v>466</v>
+      </c>
+      <c r="B199" t="s">
+        <v>467</v>
+      </c>
+      <c r="C199">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A200" t="s">
+        <v>468</v>
+      </c>
+      <c r="B200" t="s">
+        <v>469</v>
+      </c>
+      <c r="C200">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A201" t="s">
+        <v>470</v>
+      </c>
+      <c r="B201" t="s">
+        <v>471</v>
+      </c>
+      <c r="C201">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A202" t="s">
+        <v>472</v>
+      </c>
+      <c r="B202" t="s">
+        <v>473</v>
+      </c>
+      <c r="C202">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A203" t="s">
+        <v>474</v>
+      </c>
+      <c r="B203" t="s">
+        <v>475</v>
+      </c>
+      <c r="C203">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A204" t="s">
+        <v>476</v>
+      </c>
+      <c r="B204" t="s">
+        <v>477</v>
+      </c>
+      <c r="C204">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A205" t="s">
+        <v>478</v>
+      </c>
+      <c r="B205" t="s">
+        <v>479</v>
+      </c>
+      <c r="C205">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A206" t="s">
+        <v>480</v>
+      </c>
+      <c r="B206" t="s">
+        <v>481</v>
+      </c>
+      <c r="C206">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A207" t="s">
+        <v>482</v>
+      </c>
+      <c r="B207" t="s">
+        <v>483</v>
+      </c>
+      <c r="C207">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A208" t="s">
+        <v>484</v>
+      </c>
+      <c r="B208" t="s">
+        <v>485</v>
+      </c>
+      <c r="C208">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A209" t="s">
+        <v>486</v>
+      </c>
+      <c r="B209" t="s">
+        <v>487</v>
+      </c>
+      <c r="C209">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A210" t="s">
+        <v>488</v>
+      </c>
+      <c r="B210" t="s">
+        <v>489</v>
+      </c>
+      <c r="C210">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A211" t="s">
+        <v>490</v>
+      </c>
+      <c r="B211" t="s">
+        <v>491</v>
+      </c>
+      <c r="C211">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A212" t="s">
+        <v>492</v>
+      </c>
+      <c r="B212" t="s">
+        <v>493</v>
+      </c>
+      <c r="C212">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A213" t="s">
+        <v>494</v>
+      </c>
+      <c r="B213" t="s">
+        <v>495</v>
+      </c>
+      <c r="C213">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A214" t="s">
+        <v>496</v>
+      </c>
+      <c r="B214" t="s">
+        <v>497</v>
+      </c>
+      <c r="C214">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>